<commit_message>
dockerfile added for openfoam
</commit_message>
<xml_diff>
--- a/test/test_simulation_data/Resultfile.xlsx
+++ b/test/test_simulation_data/Resultfile.xlsx
@@ -1010,10 +1010,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>3.98219279472339</v>
+        <v>5.165942130649757</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>12659.84514385467</v>
+        <v>11154.18953864742</v>
       </c>
     </row>
     <row r="3">
@@ -1021,10 +1021,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>2.007347000063122</v>
+        <v>4.798849819416276</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>15673.70169019627</v>
+        <v>13672.96917189622</v>
       </c>
     </row>
   </sheetData>
@@ -1098,39 +1098,39 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>3.98219279472339</v>
+        <v>5.165942130649757</v>
       </c>
       <c r="C2" t="n">
-        <v>12659.84514385467</v>
+        <v>11154.18953864742</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>269</t>
+          <t>276</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>12659.8</t>
+          <t>11153.7</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>12662.1</t>
+          <t>11157.6</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>269</t>
+          <t>276</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2.71206</t>
+          <t>3.45664</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2.41211</t>
+          <t>3.12996</t>
         </is>
       </c>
     </row>
@@ -1139,39 +1139,39 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2.007347000063122</v>
+        <v>4.798849819416276</v>
       </c>
       <c r="C3" t="n">
-        <v>15673.70169019627</v>
+        <v>13672.96917189622</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>262</t>
+          <t>275</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>15674</t>
+          <t>13672.6</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>15674.4</t>
+          <t>13676</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>262</t>
+          <t>275</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>1.37492</t>
+          <t>3.22726</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1.19331</t>
+          <t>2.91238</t>
         </is>
       </c>
     </row>

</xml_diff>